<commit_message>
Review ERC/DRC Generate gerber, drill, schematics pdf and pick n place Update BOM Release V0
</commit_message>
<xml_diff>
--- a/H12R00/Released/BOM/H12R00.xlsx
+++ b/H12R00/Released/BOM/H12R00.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\Hardware\H12R0x-Hardware\H12R00\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H12R0x-Hardware\H12R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F15872B-A041-4D0E-8AB7-77A381B277AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-30" windowWidth="23025" windowHeight="4335"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +24,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -44,7 +45,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
   <si>
     <t>Qty</t>
   </si>
@@ -158,21 +159,6 @@
   </si>
   <si>
     <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
-  </si>
-  <si>
-    <t>FB-TDK_MMZ1608Y300B</t>
-  </si>
-  <si>
-    <t>Ferrite Beads Multi-Layer 30Ohm 25% 100MHz 1.5A 50mOhm DCR 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDK </t>
-  </si>
-  <si>
-    <t>MMZ1608Y300B</t>
-  </si>
-  <si>
-    <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
   </si>
   <si>
     <t>VLMS1300-GS08</t>
@@ -255,9 +241,6 @@
     <t>±10%</t>
   </si>
   <si>
-    <t>3-644456-2</t>
-  </si>
-  <si>
     <t>CRCW060310K0JNEB</t>
   </si>
   <si>
@@ -270,9 +253,6 @@
     <t>Thick Film Resistors - SMD 0602</t>
   </si>
   <si>
-    <t>C3, C4</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -282,9 +262,6 @@
     <t>R7</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9, C11</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -324,9 +301,6 @@
     <t>https://octopart.com/c0603c153j3gactu-kemet-12793174</t>
   </si>
   <si>
-    <t>FB1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> AD628ARZ</t>
   </si>
   <si>
@@ -336,24 +310,12 @@
     <t xml:space="preserve"> Operational amplifier</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://octopart.com/ad628arz-analog+devices-410882</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>CRCW08053K90FKEA</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw08053k90fkea-vishay-39824474</t>
-  </si>
-  <si>
-    <t>3.9kΩ</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -384,21 +346,6 @@
     <t>https://octopart.com/crcw080549r9fkea-vishay-39436139</t>
   </si>
   <si>
-    <t>PWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Connector Unshrouded Header HDR 2 Position 2.54mm Solder Straight Thru-Hole </t>
-  </si>
-  <si>
-    <t>TE Connectivity</t>
-  </si>
-  <si>
-    <t>https://www.te.com/usa-en/product-3-644456-2.html?te_bu=Cor&amp;te_type=disp&amp;te_campaign=seda_glo_cor-seda-global-disp-prtnr-fy19-seda-model-bom-cta_sma-317_1&amp;elqCampaignId=32493</t>
-  </si>
-  <si>
-    <t>Analog Input</t>
-  </si>
-  <si>
     <t>https://octopart.com/1751251-phoenix+contact-36473?r=sp&amp;s=9M0VWNoHTyq04j3qI6lQOQ</t>
   </si>
   <si>
@@ -406,12 +353,90 @@
   </si>
   <si>
     <t>Terminal Block 10 A 160 V 3.5 mm 26 to 16 AWG 2 Screw Solder 2.5 kV PA</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C8, C9, C11, C14</t>
+  </si>
+  <si>
+    <t>C4, C7</t>
+  </si>
+  <si>
+    <t>DIODES_SBR2U30P1-7</t>
+  </si>
+  <si>
+    <t>2.0A SBR SUPER BARRIER RECTIFIER POWERDI123</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>SBR2U30P1-7</t>
+  </si>
+  <si>
+    <t>https://octopart.com/sbr2u30p1-7-diodes+inc.-13160632?r=sp&amp;s=T9EzcoJOQBe5XnC2-oZtAA</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>SMBJ30CA</t>
+  </si>
+  <si>
+    <t>TVS Diode</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>https://octopart.com/smbj30ca-on+semiconductor-84331460?r=sp&amp;s=Vl5BdVYHQCeKmKgfbE4rMg</t>
+  </si>
+  <si>
+    <t>TVS1</t>
+  </si>
+  <si>
+    <t>NANOSMDC035F-2120</t>
+  </si>
+  <si>
+    <t>PTC Resettable Fuse 0.35A(hold) 0.75A(trip) 16VDC 20A 0.6W 0.1s 0.45Ohm SMD Solder Pad 1206</t>
+  </si>
+  <si>
+    <t>Littelfuse</t>
+  </si>
+  <si>
+    <t>NANOSMDC035F-2</t>
+  </si>
+  <si>
+    <t>https://octopart.com/nanosmdc035f-2-littelfuse-74215052?r=sp&amp;s=rfNZOPvgSJy5H1V-bbPI5Q#</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>PWR, Analog Input</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>REF193GSZ</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ref193gsz-analog+devices-524457#</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ad628arz-analog+devices-410882</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>Voltage Reference Precision 3 Volt 30 mA 8-Pin SOIC N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,6 +521,9 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -516,7 +544,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="H10R4" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="H10R4" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,6 +623,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -630,6 +675,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -805,35 +867,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="90.5703125" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3984375" customWidth="1"/>
+    <col min="8" max="8" width="90.59765625" customWidth="1"/>
+    <col min="9" max="9" width="6.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -845,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -854,15 +916,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -874,13 +936,13 @@
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -891,7 +953,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -906,7 +968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -914,10 +976,10 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>27</v>
@@ -932,7 +994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -940,7 +1002,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -958,192 +1020,192 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>1751251</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1">
         <v>1751251</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -1158,15 +1220,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -1182,227 +1244,247 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G16" s="4">
         <v>0.01</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G17" s="4">
         <v>0.01</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4">
         <v>0.01</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0.01</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>97</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2" t="s">
-        <v>44</v>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H9" r:id="rId3"/>
-    <hyperlink ref="H15" r:id="rId4"/>
-    <hyperlink ref="H16" r:id="rId5"/>
-    <hyperlink ref="H6" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H8" r:id="rId8"/>
-    <hyperlink ref="H4" r:id="rId9"/>
-    <hyperlink ref="H17" r:id="rId10"/>
-    <hyperlink ref="H13" r:id="rId11"/>
-    <hyperlink ref="H18" r:id="rId12"/>
-    <hyperlink ref="H19" r:id="rId13"/>
-    <hyperlink ref="H11" r:id="rId14"/>
-    <hyperlink ref="H12" r:id="rId15"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H21" r:id="rId14" xr:uid="{9E387A9A-5B66-4BE2-993D-4530C7842261}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some BOM errors
</commit_message>
<xml_diff>
--- a/H12R00/Released/BOM/H12R00.xlsx
+++ b/H12R00/Released/BOM/H12R00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H12R0x-Hardware\H12R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F15872B-A041-4D0E-8AB7-77A381B277AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E1B50-22F8-4A7B-A179-ACA159784934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,9 +307,6 @@
     <t>High Common-Mode Voltage,Programmable Gain Difference Amplifier</t>
   </si>
   <si>
-    <t xml:space="preserve"> Operational amplifier</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -431,6 +428,9 @@
   </si>
   <si>
     <t>Voltage Reference Precision 3 Volt 30 mA 8-Pin SOIC N</t>
+  </si>
+  <si>
+    <t>CRCW080510K0FKEA</t>
   </si>
 </sst>
 </file>
@@ -871,7 +871,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -924,7 +924,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -976,7 +976,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>46</v>
@@ -1127,23 +1127,23 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
@@ -1151,23 +1151,23 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
@@ -1178,20 +1178,20 @@
         <v>1751251</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1">
         <v>1751251</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
@@ -1225,10 +1225,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
@@ -1275,10 +1275,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -1287,13 +1287,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="G16" s="4">
         <v>0.01</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>56</v>
@@ -1313,13 +1313,13 @@
         <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="4">
         <v>0.01</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -1327,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>57</v>
@@ -1339,13 +1339,13 @@
         <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="4">
         <v>0.01</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -1386,14 +1386,14 @@
         <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -1401,23 +1401,23 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -1425,22 +1425,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
- Fixed labels in .sch and .brd from 12v to 10v - Regenerated docoument file - Fixed BOM - Regenerated output files (Gerber, drills, mount)
</commit_message>
<xml_diff>
--- a/H12R00/Released/BOM/H12R00.xlsx
+++ b/H12R00/Released/BOM/H12R00.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H12R0x-Hardware\H12R00\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANAS\Desktop\H12R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E1B50-22F8-4A7B-A179-ACA159784934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +23,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -45,7 +44,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -69,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="120">
   <si>
     <t>Qty</t>
   </si>
@@ -352,9 +351,6 @@
     <t>Terminal Block 10 A 160 V 3.5 mm 26 to 16 AWG 2 Screw Solder 2.5 kV PA</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9, C11, C14</t>
-  </si>
-  <si>
     <t>C4, C7</t>
   </si>
   <si>
@@ -431,12 +427,30 @@
   </si>
   <si>
     <t>CRCW080510K0FKEA</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C8, C9</t>
+  </si>
+  <si>
+    <t>C11, C14</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cc0805krx7r8bb104-yageo-39467766?r=sp</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R8BB104</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yageo</t>
+  </si>
+  <si>
+    <t>0805 100nF 25 V ±10 % Tolerance X7R SMT Multilayer Ceramic Capacitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,7 +558,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="H10R4" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="H10R4" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,23 +637,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -675,23 +672,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -867,27 +847,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.265625" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" customWidth="1"/>
-    <col min="8" max="8" width="90.59765625" customWidth="1"/>
-    <col min="9" max="9" width="6.265625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="90.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -916,15 +896,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -942,343 +922,343 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="G5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A12" s="1">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1751251</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1751251</v>
+        <v>102</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1751251</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1751251</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.01</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.65" x14ac:dyDescent="0.5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -1287,24 +1267,24 @@
         <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0.01</v>
+        <v>51</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -1313,24 +1293,24 @@
         <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="G17" s="4">
         <v>0.01</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -1345,144 +1325,170 @@
         <v>0.01</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2" t="s">
+      <c r="G24" s="1"/>
+      <c r="H24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H21" r:id="rId14" xr:uid="{9E387A9A-5B66-4BE2-993D-4530C7842261}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H10" r:id="rId3"/>
+    <hyperlink ref="H16" r:id="rId4"/>
+    <hyperlink ref="H7" r:id="rId5"/>
+    <hyperlink ref="H8" r:id="rId6"/>
+    <hyperlink ref="H9" r:id="rId7"/>
+    <hyperlink ref="H5" r:id="rId8"/>
+    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H14" r:id="rId10"/>
+    <hyperlink ref="H18" r:id="rId11"/>
+    <hyperlink ref="H19" r:id="rId12"/>
+    <hyperlink ref="H13" r:id="rId13"/>
+    <hyperlink ref="H22" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
- Made some Hardware modifications (.sch and .brd where updated) - Updated Documentation - Updated BOM - Regenerated output files
</commit_message>
<xml_diff>
--- a/H12R00/Released/BOM/H12R00.xlsx
+++ b/H12R00/Released/BOM/H12R00.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="126">
   <si>
     <t>Qty</t>
   </si>
@@ -315,15 +315,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw080510k0fkea-vishay-39436722</t>
-  </si>
-  <si>
-    <t>15KΩ</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
     <t>10.0kΩ</t>
   </si>
   <si>
@@ -333,9 +324,6 @@
     <t>270.0Ω</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw080515k0fkea-vishay-39456030</t>
-  </si>
-  <si>
     <t>49.9Ω</t>
   </si>
   <si>
@@ -408,43 +396,73 @@
     <t>PWR, Analog Input</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>REF193GSZ</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ref193gsz-analog+devices-524457#</t>
-  </si>
-  <si>
     <t>https://octopart.com/ad628arz-analog+devices-410882</t>
   </si>
   <si>
     <t>Analog Devices</t>
   </si>
   <si>
-    <t>Voltage Reference Precision 3 Volt 30 mA 8-Pin SOIC N</t>
-  </si>
-  <si>
-    <t>CRCW080510K0FKEA</t>
-  </si>
-  <si>
     <t>C3, C5, C6, C8, C9</t>
   </si>
   <si>
-    <t>C11, C14</t>
-  </si>
-  <si>
-    <t>https://octopart.com/cc0805krx7r8bb104-yageo-39467766?r=sp</t>
-  </si>
-  <si>
-    <t>CC0805KRX7R8BB104</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yageo</t>
-  </si>
-  <si>
-    <t>0805 100nF 25 V ±10 % Tolerance X7R SMT Multilayer Ceramic Capacitor</t>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>https://octopart.com/erj-2rkf6202x-panasonic-55404988?r=sp</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF6202X</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0402 62K Ohm 1% 0.1W(1/10W) +/-100ppm/C Molded SMD Automotive Punched T/R</t>
+  </si>
+  <si>
+    <t>62kΩ</t>
+  </si>
+  <si>
+    <t>51kΩ</t>
+  </si>
+  <si>
+    <t>https://octopart.com/smbj3v3-e3%2F52-vishay-39558764?r=sp</t>
+  </si>
+  <si>
+    <t>SMBJ3V3-E3/52</t>
+  </si>
+  <si>
+    <t>TVS2, TVS3</t>
+  </si>
+  <si>
+    <t>SMBJ Series 600 W 7.3 V Uni Directional Surface Mount TVS Diode - DO-214AA</t>
+  </si>
+  <si>
+    <t>https://octopart.com/erj-2rkf5102x-panasonic-42799737?r=sp</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF5102X</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0402 51K Ohm 1% 0.1W(1/10W) +/-100ppm/C Molded SMD Automotive Punched T/R</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 0.01uF 50V X7R 10% Pad SMD 0603 125°C T/R</t>
+  </si>
+  <si>
+    <t>22KΩ</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rt0603fre0722kl-yageo-40031569?r=sp</t>
+  </si>
+  <si>
+    <t>High Precision-High Stability Chip Resistor Thin Film 0603 High Precision-High Stability Chip Resistor Thin Film 0603 22kOhm 1% Paper T/R</t>
+  </si>
+  <si>
+    <t>RT0603FRE0722KL</t>
   </si>
 </sst>
 </file>
@@ -494,7 +512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -517,12 +535,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -539,6 +583,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -848,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +910,7 @@
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
@@ -904,7 +955,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -924,28 +975,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -982,7 +1033,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>46</v>
@@ -1133,23 +1184,23 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1157,23 +1208,23 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1184,20 +1235,20 @@
         <v>1751251</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F13" s="1">
         <v>1751251</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -1231,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>73</v>
@@ -1255,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
@@ -1281,25 +1332,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G17" s="4">
         <v>0.01</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1307,25 +1358,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="G18" s="4">
         <v>0.01</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1333,25 +1384,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="G19" s="4">
         <v>0.01</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1359,23 +1410,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.01</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,23 +1436,23 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="2" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1407,23 +1460,23 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,45 +1484,70 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="G23" s="8"/>
       <c r="H23" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1483,14 +1561,16 @@
     <hyperlink ref="H8" r:id="rId6"/>
     <hyperlink ref="H9" r:id="rId7"/>
     <hyperlink ref="H5" r:id="rId8"/>
-    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId9"/>
     <hyperlink ref="H14" r:id="rId10"/>
-    <hyperlink ref="H18" r:id="rId11"/>
-    <hyperlink ref="H19" r:id="rId12"/>
+    <hyperlink ref="H19" r:id="rId11"/>
+    <hyperlink ref="H20" r:id="rId12"/>
     <hyperlink ref="H13" r:id="rId13"/>
-    <hyperlink ref="H22" r:id="rId14"/>
+    <hyperlink ref="H17" r:id="rId14"/>
+    <hyperlink ref="H24" r:id="rId15"/>
+    <hyperlink ref="H3" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Fix some documentation issues
</commit_message>
<xml_diff>
--- a/H12R00/Released/BOM/H12R00.xlsx
+++ b/H12R00/Released/BOM/H12R00.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H12R0x-Hardware\H12R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC07597D-9A42-401E-A600-D3451567EFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2F6D74-6CF8-425B-88AC-31D78B343BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H26R01" sheetId="1" r:id="rId1"/>
+    <sheet name="H12R00" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="137">
   <si>
     <t>Description</t>
   </si>
@@ -211,15 +211,6 @@
     <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
   </si>
   <si>
-    <t>CAP CER 10UF 10V X5R 0603</t>
-  </si>
-  <si>
-    <t>GRM188R61A106KE69D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm188r61a106ke69d-murata-22851381?r=ap&amp;s=o9t4ILLiSny6rfdd0oM5Kg</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve"> SWD</t>
-  </si>
-  <si>
-    <t>C9, C10, C13, C17, C19</t>
   </si>
   <si>
     <t>https://octopart.com/1984646-phoenix+contact-50274?r=sp&amp;s=drI_GVM4QHaL48lSCATrxQ</t>
@@ -460,12 +448,33 @@
   <si>
     <t xml:space="preserve">Industrial Analog I/P ±10 V  (H12R00) </t>
   </si>
+  <si>
+    <t>C10 , C11</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10 uF 35 VDC 20% 0805 X5R</t>
+  </si>
+  <si>
+    <t>GRM21BR6YA106ME43K</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>https://octopart.com/grm21br6ya106me43k-murata-57368791?r=sp</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0710kl-yageo-40025538?r=sp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,12 +517,6 @@
     </font>
     <font>
       <b/>
-      <sz val="28"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -687,7 +690,7 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -1064,49 +1067,49 @@
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1114,48 +1117,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1179,14 +1172,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1264,7 +1254,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2174599</xdr:colOff>
+      <xdr:colOff>2108338</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
@@ -1606,17 +1596,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="1" max="1" width="13.59765625" customWidth="1"/>
     <col min="2" max="2" width="70.59765625" customWidth="1"/>
     <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
@@ -1628,8 +1618,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1639,8 +1628,8 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1652,11 +1641,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="15">
         <v>0</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1669,11 +1658,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="16">
         <v>45229</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1681,14 +1670,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1698,10 +1687,10 @@
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1711,503 +1700,503 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1984646</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="16">
+      <c r="B21" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="16">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="15">
-        <v>1984646</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="16">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="16">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="16">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="16">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="16">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="15" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2218,21 +2207,20 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
+    <hyperlink ref="E21" r:id="rId2" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E33" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E27" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E33" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
-    <hyperlink ref="E25" r:id="rId11" xr:uid="{8247B2C4-59B6-4E38-8F18-15A37292F9D6}"/>
-    <hyperlink ref="E12" r:id="rId12" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
+    <hyperlink ref="E30" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E26" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
-  <drawing r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>